<commit_message>
Updated Team Info (Only contains name, email, and role)
Team information is provided in case any member needs to get in contact
with one another during development.
</commit_message>
<xml_diff>
--- a/TeamInfo/Teamdevs.xlsx
+++ b/TeamInfo/Teamdevs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
   <si>
     <t>Game Development Project</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Developer/Art Design/Level Design</t>
   </si>
   <si>
-    <t xml:space="preserve"> Developer/Animator/Art Designer/Level Design</t>
-  </si>
-  <si>
     <t>ConnorAHaskins@gmail.com</t>
   </si>
   <si>
@@ -114,16 +111,25 @@
     <t>Andrew</t>
   </si>
   <si>
-    <t>Ashley</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Animators/ Story board / </t>
-  </si>
-  <si>
     <t>Developer Backend ?</t>
   </si>
   <si>
-    <t>Lead Developer Backend</t>
+    <t>Ashleigh "Lee" Rinkle</t>
+  </si>
+  <si>
+    <t>Lead Developer Backend/ Story Board</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lead Art Director/Animator/ Story Board  </t>
+  </si>
+  <si>
+    <t>Project Manager/ Developer/ Art Design</t>
+  </si>
+  <si>
+    <t>Toolsets</t>
+  </si>
+  <si>
+    <t>Team Info</t>
   </si>
 </sst>
 </file>
@@ -551,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -572,12 +578,15 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J4" s="5" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J4" s="5" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -591,7 +600,7 @@
         <v>3</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -599,13 +608,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -613,13 +622,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -627,13 +636,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -641,13 +650,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -655,7 +664,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>13</v>
@@ -666,7 +675,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>11</v>
@@ -677,7 +686,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>14</v>
@@ -685,16 +694,16 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -707,7 +716,12 @@
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some changes in roles for team
</commit_message>
<xml_diff>
--- a/TeamInfo/Teamdevs.xlsx
+++ b/TeamInfo/Teamdevs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Game Development Project</t>
   </si>
@@ -54,12 +54,6 @@
     <t>Developer Backend</t>
   </si>
   <si>
-    <t>Developer/Music/Level Design</t>
-  </si>
-  <si>
-    <t>Developer/Art Design/Animator</t>
-  </si>
-  <si>
     <t>Developer/Art Design/Level Design</t>
   </si>
   <si>
@@ -130,6 +124,15 @@
   </si>
   <si>
     <t>Team Info</t>
+  </si>
+  <si>
+    <t>Developer/Art Design/Animator/Music/Story Board Director/Writer</t>
+  </si>
+  <si>
+    <t>Developer/Music/Level Design/Writer/</t>
+  </si>
+  <si>
+    <t>Developer Backend/Lead Programmer</t>
   </si>
 </sst>
 </file>
@@ -560,14 +563,14 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" customWidth="1"/>
     <col min="2" max="2" width="29.5703125" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" customWidth="1"/>
+    <col min="3" max="3" width="60.28515625" customWidth="1"/>
     <col min="10" max="10" width="24.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -578,15 +581,15 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -600,7 +603,7 @@
         <v>3</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -608,13 +611,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -622,13 +625,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -636,13 +639,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -650,13 +653,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>12</v>
+        <v>37</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -664,10 +667,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>13</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -675,10 +678,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -686,24 +689,24 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="4" t="s">
@@ -712,16 +715,16 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>